<commit_message>
updating with the GUI interface & adding files that have been updated since I moved
</commit_message>
<xml_diff>
--- a/python_wrapper/optimization_runs/Aug17_2021/run2.xlsx
+++ b/python_wrapper/optimization_runs/Aug17_2021/run2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patla\Desktop\Thermal_Laser_Compression_Model\python_wrapper\optimization_runs\Aug17_2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plachap1\Thermal_Laser_Compression_Model\python_wrapper\optimization_runs\Aug17_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E47F630-95B0-459B-99E5-63EA0C6B672D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A44E5D-9903-40C0-B67A-6A28A87C4136}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E10B1A3E-F900-4A8C-BCBA-C8576F221F40}"/>
   </bookViews>
@@ -20,23 +20,32 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>iteration</t>
+  </si>
+  <si>
+    <t>SLS</t>
+  </si>
+  <si>
+    <t>peak_temp</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>time_shift</t>
+  </si>
+  <si>
+    <t>diffusivity</t>
   </si>
 </sst>
 </file>
@@ -180,6 +189,9 @@
               <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SLS</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1089,6 +1101,9 @@
               <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>peak_temp</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1973,6 +1988,9 @@
               <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2882,6 +2900,9 @@
               <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -3766,6 +3787,9 @@
               <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time_shift</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -4650,6 +4674,9 @@
               <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>diffusivity</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -5719,46 +5746,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8335,557 +8322,6 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -9410,18 +8846,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99247D8B-4D68-40BB-8A9A-53D51BB14844}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G152"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9444,7 +8898,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -9468,7 +8922,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
@@ -9492,7 +8946,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -9516,7 +8970,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -9540,7 +8994,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -9564,7 +9018,7 @@
         <v>37800000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -9588,7 +9042,7 @@
         <v>36720000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -9612,7 +9066,7 @@
         <v>37080000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -9636,7 +9090,7 @@
         <v>37152000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -9660,7 +9114,7 @@
         <v>37612800</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -9684,7 +9138,7 @@
         <v>38419200</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -9708,7 +9162,7 @@
         <v>36060480</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -9732,7 +9186,7 @@
         <v>35190720</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -9756,7 +9210,7 @@
         <v>37536768</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -9780,7 +9234,7 @@
         <v>38151475.200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -9804,7 +9258,7 @@
         <v>37399265.280000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -9828,7 +9282,7 @@
         <v>37522897.920000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -9852,7 +9306,7 @@
         <v>37648424.447999999</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -9876,7 +9330,7 @@
         <v>37932636.671999902</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -9900,7 +9354,7 @@
         <v>36000914.227200001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -9924,7 +9378,7 @@
         <v>34791771.340800002</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -9948,7 +9402,7 @@
         <v>36269004.718079999</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -9972,7 +9426,7 @@
         <v>35635123.077119999</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -9996,7 +9450,7 @@
         <v>34901309.325311899</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -10020,7 +9474,7 @@
         <v>37746300.255436704</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -10044,7 +9498,7 @@
         <v>35829615.063859098</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -10068,7 +9522,7 @@
         <v>38407033.225543603</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -10092,7 +9546,7 @@
         <v>35777740.300369903</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -10116,7 +9570,7 @@
         <v>37457977.581600703</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -10140,7 +9594,7 @@
         <v>36236705.693294503</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -10164,7 +9618,7 @@
         <v>35250217.834777802</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -10188,7 +9642,7 @@
         <v>36784366.468171</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -10212,7 +9666,7 @@
         <v>37925548.387120403</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -10236,7 +9690,7 @@
         <v>35919050.472863398</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -10260,7 +9714,7 @@
         <v>36811998.4404312</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -10284,7 +9738,7 @@
         <v>35065709.282698303</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10308,7 +9762,7 @@
         <v>35203619.627173901</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10332,7 +9786,7 @@
         <v>34399430.220545202</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10356,7 +9810,7 @@
         <v>35695786.000394598</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10380,7 +9834,7 @@
         <v>35543221.886992</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10404,7 +9858,7 @@
         <v>36821995.986613803</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -10428,7 +9882,7 @@
         <v>35118390.608518198</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -10452,7 +9906,7 @@
         <v>35663442.658087701</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -10476,7 +9930,7 @@
         <v>35535638.7506999</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -10500,7 +9954,7 @@
         <v>36631001.7793056</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -10524,7 +9978,7 @@
         <v>35625186.4942341</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -10548,7 +10002,7 @@
         <v>34593471.428748302</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -10572,7 +10026,7 @@
         <v>33479209.1498156</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -10596,7 +10050,7 @@
         <v>35522083.597245</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -10620,7 +10074,7 @@
         <v>35681315.582280599</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -10644,7 +10098,7 @@
         <v>33714826.966303296</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -10668,7 +10122,7 @@
         <v>33956498.4402024</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -10692,7 +10146,7 @@
         <v>33403773.668728702</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -10716,7 +10170,7 @@
         <v>32334049.559597101</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -10740,7 +10194,7 @@
         <v>32558610.772232398</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -10764,7 +10218,7 @@
         <v>31070096.782998599</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -10788,7 +10242,7 @@
         <v>33651395.426389903</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -10812,7 +10266,7 @@
         <v>33052064.930477999</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -10836,7 +10290,7 @@
         <v>33730390.062771298</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -10860,7 +10314,7 @@
         <v>33299961.6429644</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -10884,7 +10338,7 @@
         <v>30380931.4512606</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -10908,7 +10362,7 @@
         <v>27730739.385750499</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -10932,7 +10386,7 @@
         <v>30992073.5261655</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -10956,7 +10410,7 @@
         <v>33045810.928619899</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -10980,7 +10434,7 @@
         <v>31175504.824164599</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -11004,7 +10458,7 @@
         <v>30429534.122409102</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <f t="shared" ref="A68:A100" si="1">A67+1</f>
         <v>66</v>
@@ -11028,7 +10482,7 @@
         <v>28994320.362131398</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -11052,7 +10506,7 @@
         <v>29637174.114269201</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -11076,7 +10530,7 @@
         <v>30489333.3178569</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -11100,7 +10554,7 @@
         <v>27766764.773086101</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -11124,7 +10578,7 @@
         <v>24824449.4464342</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -11148,7 +10602,7 @@
         <v>28879159.354879901</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -11172,7 +10626,7 @@
         <v>28108192.424798299</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -11196,7 +10650,7 @@
         <v>26627240.245698199</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -11220,7 +10674,7 @@
         <v>27144118.661076602</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -11244,7 +10698,7 @@
         <v>28060276.3465323</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -11268,7 +10722,7 @@
         <v>25630242.208260302</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -11292,7 +10746,7 @@
         <v>23661922.771452401</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -11316,7 +10770,7 @@
         <v>25554459.876935098</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -11340,7 +10794,7 @@
         <v>26746703.965041202</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -11364,7 +10818,7 @@
         <v>24523789.4417077</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -11388,7 +10842,7 @@
         <v>22815683.106331602</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -11412,7 +10866,7 @@
         <v>26749128.036482099</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -11436,7 +10890,7 @@
         <v>24130225.116399098</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -11460,7 +10914,7 @@
         <v>22821985.692078002</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -11484,7 +10938,7 @@
         <v>24646680.0364355</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -11508,7 +10962,7 @@
         <v>25384351.665304098</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -11532,7 +10986,7 @@
         <v>27303971.0307841</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -11556,7 +11010,7 @@
         <v>24572434.836285301</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -11580,7 +11034,7 @@
         <v>26461562.518359799</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -11604,7 +11058,7 @@
         <v>25008232.710870702</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -11628,7 +11082,7 @@
         <v>23710508.700438399</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -11652,7 +11106,7 @@
         <v>22252142.9278084</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -11676,7 +11130,7 @@
         <v>21789826.866184901</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -11700,7 +11154,7 @@
         <v>19310176.281036299</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -11724,7 +11178,7 @@
         <v>21716793.317715298</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -11748,7 +11202,7 @@
         <v>24467462.0784069</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -11772,7 +11226,7 @@
         <v>22486721.0435827</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -11796,7 +11250,7 @@
         <v>21042318.502082098</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B101">
         <v>23775048639.197399</v>
       </c>
@@ -11816,7 +11270,7 @@
         <v>22033797.054279301</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B102">
         <v>23745299300.508999</v>
       </c>
@@ -11836,7 +11290,7 @@
         <v>21081754.8717058</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B103">
         <v>23802767841.4062</v>
       </c>
@@ -11856,7 +11310,7 @@
         <v>19390235.027017601</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B104">
         <v>23743819091.375801</v>
       </c>
@@ -11876,7 +11330,7 @@
         <v>20659541.789864901</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B105">
         <v>23761730871.415798</v>
       </c>
@@ -11896,7 +11350,7 @@
         <v>21274197.945379499</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B106">
         <v>23835914746.135502</v>
       </c>
@@ -11916,7 +11370,7 @@
         <v>20664674.078878701</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B107">
         <v>23732497275.595001</v>
       </c>
@@ -11936,7 +11390,7 @@
         <v>21855275.715576001</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B108">
         <v>23756391528.983501</v>
       </c>
@@ -11956,7 +11410,7 @@
         <v>21875050.169386301</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B109">
         <v>23770012385.833302</v>
       </c>
@@ -11976,7 +11430,7 @@
         <v>20417858.721504401</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B110">
         <v>23736775034.152599</v>
       </c>
@@ -11996,7 +11450,7 @@
         <v>21969505.463063199</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B111">
         <v>23746605602.425598</v>
       </c>
@@ -12016,7 +11470,7 @@
         <v>21067311.713171698</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B112">
         <v>23731323942.960602</v>
       </c>
@@ -12036,7 +11490,7 @@
         <v>21269246.327225301</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B113">
         <v>23777343458.990601</v>
       </c>
@@ -12056,7 +11510,7 @@
         <v>21935603.593059901</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B114">
         <v>23729423200.420799</v>
       </c>
@@ -12076,7 +11530,7 @@
         <v>21295217.052044399</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B115">
         <v>23760377915.620899</v>
       </c>
@@ -12096,7 +11550,7 @@
         <v>22612086.779772598</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B116">
         <v>23729687507.406601</v>
       </c>
@@ -12116,7 +11570,7 @@
         <v>21147678.0373418</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B117">
         <v>23733039562.856499</v>
       </c>
@@ -12136,7 +11590,7 @@
         <v>21224942.1719153</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B118">
         <v>23719440574.501499</v>
       </c>
@@ -12156,7 +11610,7 @@
         <v>20747438.258577999</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B119">
         <v>23716966600.7188</v>
       </c>
@@ -12176,7 +11630,7 @@
         <v>20136404.656335399</v>
       </c>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B120">
         <v>23728739439.493301</v>
       </c>
@@ -12196,7 +11650,7 @@
         <v>21056586.5434938</v>
       </c>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B121">
         <v>23723658089.549198</v>
       </c>
@@ -12216,7 +11670,7 @@
         <v>20106777.331000298</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B122">
         <v>23725915126.4981</v>
       </c>
@@ -12236,7 +11690,7 @@
         <v>20227819.120860901</v>
       </c>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B123">
         <v>23710934228.025299</v>
       </c>
@@ -12256,7 +11710,7 @@
         <v>19981443.8441521</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B124">
         <v>23705588422.362</v>
       </c>
@@ -12276,7 +11730,7 @@
         <v>19398326.7475572</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B125">
         <v>23723467927.430801</v>
       </c>
@@ -12296,7 +11750,7 @@
         <v>19075148.7076547</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B126">
         <v>23719092899.122799</v>
       </c>
@@ -12316,7 +11770,7 @@
         <v>18521204.081869598</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B127">
         <v>23717358947.8484</v>
       </c>
@@ -12336,7 +11790,7 @@
         <v>18667325.488905899</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B128">
         <v>23705418629.611198</v>
       </c>
@@ -12356,7 +11810,7 @@
         <v>18212586.541928802</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B129">
         <v>23707978912.5028</v>
       </c>
@@ -12376,7 +11830,7 @@
         <v>17265491.1473931</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B130">
         <v>23729385992.665501</v>
       </c>
@@ -12396,7 +11850,7 @@
         <v>18899190.298984099</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B131">
         <v>23712063162.054699</v>
       </c>
@@ -12416,7 +11870,7 @@
         <v>19031159.105487</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B132">
         <v>23702186546.204399</v>
       </c>
@@ -12436,7 +11890,7 @@
         <v>19657116.934216201</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B133">
         <v>23704513964.441898</v>
       </c>
@@ -12456,7 +11910,7 @@
         <v>20225073.360389501</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B134">
         <v>23719009128.301998</v>
       </c>
@@ -12476,7 +11930,7 @@
         <v>19906912.105303898</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B135">
         <v>23708641391.499699</v>
       </c>
@@ -12496,7 +11950,7 @@
         <v>18977222.143005401</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B136">
         <v>23692910246.871498</v>
       </c>
@@ -12516,7 +11970,7 @@
         <v>17974159.932542499</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B137">
         <v>23683739141.8456</v>
       </c>
@@ -12536,7 +11990,7 @@
         <v>16893037.570645999</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B138">
         <v>23691984658.381302</v>
       </c>
@@ -12556,7 +12010,7 @@
         <v>18224156.869454399</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B139">
         <v>23680558940.662102</v>
       </c>
@@ -12576,7 +12030,7 @@
         <v>17976867.722515602</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B140">
         <v>23667262125.7831</v>
       </c>
@@ -12596,7 +12050,7 @@
         <v>17476690.5122707</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B141">
         <v>23674169251.294899</v>
       </c>
@@ -12616,7 +12070,7 @@
         <v>16787108.623849299</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B142">
         <v>23666926387.235901</v>
       </c>
@@ -12636,7 +12090,7 @@
         <v>17402657.662245799</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B143">
         <v>23661244697.4119</v>
       </c>
@@ -12656,7 +12110,7 @@
         <v>16997693.222404301</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B144">
         <v>23651174061.484901</v>
       </c>
@@ -12676,7 +12130,7 @@
         <v>14894357.785233701</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B145">
         <v>23640858536.978001</v>
       </c>
@@ -12696,7 +12150,7 @@
         <v>12512978.2107425</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B146">
         <v>23624077656.282398</v>
       </c>
@@ -12716,7 +12170,7 @@
         <v>14042846.3865107</v>
       </c>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B147">
         <v>23591149018.328201</v>
       </c>
@@ -12736,7 +12190,7 @@
         <v>11952191.145038901</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B148">
         <v>23595838647.206501</v>
       </c>
@@ -12756,7 +12210,7 @@
         <v>13397627.1150763</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B149">
         <v>23598932726.9809</v>
       </c>
@@ -12776,7 +12230,7 @@
         <v>12147763.458363799</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B150">
         <v>23579699967.407398</v>
       </c>
@@ -12796,7 +12250,7 @@
         <v>9326610.7483795807</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B151">
         <v>23506289316.151199</v>
       </c>
@@ -12816,7 +12270,7 @@
         <v>5251570.8664339697</v>
       </c>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B152">
         <v>23493426122.5434</v>
       </c>

</xml_diff>